<commit_message>
Completed Working with the MIN() and MAX() functions
</commit_message>
<xml_diff>
--- a/04 - Basic Excel Functions/MonthlyBudget.xlsx
+++ b/04 - Basic Excel Functions/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/04 - Basic Excel Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91013AF8-BD11-4381-8FC6-388864D0CE60}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A475B7A9-474A-4372-AE14-94FB787A950B}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>Percent</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
   </si>
 </sst>
 </file>
@@ -384,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -558,6 +567,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>MIN(B4:B8)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f>MAX(B4:B8)</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Completed Working with the AVERAGE() function
</commit_message>
<xml_diff>
--- a/04 - Basic Excel Functions/MonthlyBudget.xlsx
+++ b/04 - Basic Excel Functions/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/04 - Basic Excel Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A475B7A9-474A-4372-AE14-94FB787A950B}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0963B07-217D-477E-B53A-5D1E803A62DB}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,6 +575,14 @@
         <f>MIN(B4:B8)</f>
         <v>100</v>
       </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="3">MIN(C4:C8)</f>
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -584,16 +592,36 @@
         <f>MAX(B4:B8)</f>
         <v>1200</v>
       </c>
+      <c r="C12">
+        <f t="shared" ref="C12:D12" si="4">MAX(C4:C8)</f>
+        <v>1200</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <f>AVERAGE(B4:B8)</f>
+        <v>370</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:D13" si="5">AVERAGE(C4:C8)</f>
+        <v>382</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="5"/>
+        <v>337</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B9 C9:D9" formulaRange="1"/>
+    <ignoredError sqref="B9 C9:D9 B11:D13" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Working with the COUNT() Function
</commit_message>
<xml_diff>
--- a/04 - Basic Excel Functions/MonthlyBudget.xlsx
+++ b/04 - Basic Excel Functions/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/04 - Basic Excel Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0963B07-217D-477E-B53A-5D1E803A62DB}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F2B6F2F-2219-41DC-A41B-3F7ED94153A2}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>COUNT</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,10 +621,27 @@
         <v>337</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>COUNT(B4:B8)</f>
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:D14" si="6">COUNT(C4:C8)</f>
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B9 C9:D9 B11:D13" formulaRange="1"/>
+    <ignoredError sqref="B9 C9:D9 B11:D13 B14:D14" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Changing the Width and Height of Cells
</commit_message>
<xml_diff>
--- a/04 - Basic Excel Functions/MonthlyBudget.xlsx
+++ b/04 - Basic Excel Functions/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/04 - Basic Excel Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F2B6F2F-2219-41DC-A41B-3F7ED94153A2}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{319D23B2-3CE6-4445-9076-0D6EFC19B61F}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,16 +398,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>